<commit_message>
generation of Mutare data files.
</commit_message>
<xml_diff>
--- a/Project 1 -/Data_files/Cities/Mutare/Datafiles/Loan Given Report - Mutare 29 08 2022.xlsx
+++ b/Project 1 -/Data_files/Cities/Mutare/Datafiles/Loan Given Report - Mutare 29 08 2022.xlsx
@@ -1,28 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faith Kabanda\OneDrive\Documents\Data Analysis Portfolio By Faith Kabanda\Data-Analyst-Portfolio-By-Faith-Kabanda\Project 1 -\Data_files\Cities\Mutare\Datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D984CE-A339-4F23-8673-7C3513E508F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4B6BB5-1568-4362-B1EA-F2D1E5CF44C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="814" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
     <sheet name="Loans given" sheetId="2" r:id="rId2"/>
     <sheet name="Loan given repayments" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
   <si>
     <t>Respondent ID</t>
   </si>
@@ -48,18 +58,9 @@
     <t>Marital Status</t>
   </si>
   <si>
-    <t>Country of Residence</t>
-  </si>
-  <si>
     <t>Citizenship</t>
   </si>
   <si>
-    <t>Sibanda Brian</t>
-  </si>
-  <si>
-    <t>briansibanda206@gmail.com</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -69,117 +70,15 @@
     <t>Zimbabwe</t>
   </si>
   <si>
-    <t>Mary Anne Asima</t>
-  </si>
-  <si>
-    <t>asimamaryanne110@gmail.com</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
     <t>Widowed</t>
   </si>
   <si>
-    <t>Nobert Ncube</t>
-  </si>
-  <si>
-    <t>noberllasuperette@gmail.com</t>
-  </si>
-  <si>
     <t>Married</t>
   </si>
   <si>
-    <t>Clement Moyo</t>
-  </si>
-  <si>
-    <t>clementmoyo055@gmail.com</t>
-  </si>
-  <si>
-    <t>Tholakele Tshuma</t>
-  </si>
-  <si>
-    <t>tholakeletshuma123@gmail.com</t>
-  </si>
-  <si>
-    <t>Moyo Gibson</t>
-  </si>
-  <si>
-    <t>gibsgaipg@gmail.com</t>
-  </si>
-  <si>
-    <t>Mashavira Tinashe</t>
-  </si>
-  <si>
-    <t>Mashaviramashax@gmail.com</t>
-  </si>
-  <si>
-    <t>Mqabuko Nyoni</t>
-  </si>
-  <si>
-    <t>nmqabuko87@gmail.com</t>
-  </si>
-  <si>
-    <t>Mlungisi Bhebhe</t>
-  </si>
-  <si>
-    <t>mbhebhe74@gmail.com</t>
-  </si>
-  <si>
-    <t>Runesu Mupambo</t>
-  </si>
-  <si>
-    <t>runesumupambo@gmail.com</t>
-  </si>
-  <si>
-    <t>Honest Ndlovu</t>
-  </si>
-  <si>
-    <t>nhonest305@gmail.com</t>
-  </si>
-  <si>
-    <t>Linda Ncube</t>
-  </si>
-  <si>
-    <t>ncubelinda932@gmail.com</t>
-  </si>
-  <si>
-    <t>Ezweni Mabena</t>
-  </si>
-  <si>
-    <t>ezwenimabena@gmail.com</t>
-  </si>
-  <si>
-    <t>Artwell Dube</t>
-  </si>
-  <si>
-    <t>dubeartwell03@gmail.com</t>
-  </si>
-  <si>
-    <t>Bhekimpilo Mpofu</t>
-  </si>
-  <si>
-    <t>bhekimpilompofu605@gmail.com</t>
-  </si>
-  <si>
-    <t>Patrick Makonye</t>
-  </si>
-  <si>
-    <t>patrickmakonye@gmail.com</t>
-  </si>
-  <si>
-    <t>Sibusisiwe Dube</t>
-  </si>
-  <si>
-    <t>sibusisiwedube815@gmail.com</t>
-  </si>
-  <si>
-    <t>Saviour Bvute</t>
-  </si>
-  <si>
-    <t>bvutesaviour96@gmail.com</t>
-  </si>
-  <si>
     <t>+263717774729</t>
   </si>
   <si>
@@ -277,6 +176,153 @@
   </si>
   <si>
     <t>Loan given repayment report tag</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Noby</t>
+  </si>
+  <si>
+    <t>Moyo</t>
+  </si>
+  <si>
+    <t>Tshuma</t>
+  </si>
+  <si>
+    <t>Gibson</t>
+  </si>
+  <si>
+    <t>Tinashe</t>
+  </si>
+  <si>
+    <t>Nyoni</t>
+  </si>
+  <si>
+    <t>Bhebhe</t>
+  </si>
+  <si>
+    <t>Runesu</t>
+  </si>
+  <si>
+    <t>Ndlovu</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>Mabena</t>
+  </si>
+  <si>
+    <t>Artwell</t>
+  </si>
+  <si>
+    <t>Mpofu</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Sibusisiwe</t>
+  </si>
+  <si>
+    <t>Saviour</t>
+  </si>
+  <si>
+    <t>b6@xmail.com</t>
+  </si>
+  <si>
+    <t>a0@xmail.com</t>
+  </si>
+  <si>
+    <t>ne@xmail.com</t>
+  </si>
+  <si>
+    <t>c5@xmail.com</t>
+  </si>
+  <si>
+    <t>t3@xmail.com</t>
+  </si>
+  <si>
+    <t>gb@xmail.com</t>
+  </si>
+  <si>
+    <t>Mx@xmail.com</t>
+  </si>
+  <si>
+    <t>n7@gmail.com</t>
+  </si>
+  <si>
+    <t>m4@xmail.com</t>
+  </si>
+  <si>
+    <t>ru@xmail.com</t>
+  </si>
+  <si>
+    <t>254525</t>
+  </si>
+  <si>
+    <t>254738</t>
+  </si>
+  <si>
+    <t>254858</t>
+  </si>
+  <si>
+    <t>254962</t>
+  </si>
+  <si>
+    <t>255028</t>
+  </si>
+  <si>
+    <t>255260</t>
+  </si>
+  <si>
+    <t>255540</t>
+  </si>
+  <si>
+    <t>257733</t>
+  </si>
+  <si>
+    <t>257846</t>
+  </si>
+  <si>
+    <t>257945</t>
+  </si>
+  <si>
+    <t>259836</t>
+  </si>
+  <si>
+    <t>260344</t>
+  </si>
+  <si>
+    <t>261135</t>
+  </si>
+  <si>
+    <t>261423</t>
+  </si>
+  <si>
+    <t>261529</t>
+  </si>
+  <si>
+    <t>261864</t>
+  </si>
+  <si>
+    <t>261923</t>
+  </si>
+  <si>
+    <t>262026</t>
+  </si>
+  <si>
+    <t>357426</t>
+  </si>
+  <si>
+    <t>City of Residence</t>
+  </si>
+  <si>
+    <t>Mutare</t>
   </si>
 </sst>
 </file>
@@ -663,11 +709,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,24 +741,24 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2545</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2">
         <v>25</v>
@@ -719,27 +767,27 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2547</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>38</v>
@@ -748,27 +796,27 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2548</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>58</v>
@@ -777,27 +825,27 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2549</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>62</v>
@@ -806,27 +854,27 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2550</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>28</v>
@@ -835,27 +883,27 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2552</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>60</v>
@@ -864,27 +912,27 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2555</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>40</v>
@@ -893,27 +941,27 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2577</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>33</v>
@@ -922,27 +970,27 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2578</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>46</v>
@@ -951,27 +999,27 @@
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2579</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>85</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>45</v>
@@ -980,27 +1028,24 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2598</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>36</v>
@@ -1009,27 +1054,24 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2603</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <v>44</v>
@@ -1038,27 +1080,24 @@
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2611</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>88</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>35</v>
@@ -1067,27 +1106,24 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I14" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2614</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F15">
         <v>23</v>
@@ -1096,27 +1132,24 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2615</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>29</v>
@@ -1125,27 +1158,24 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>2618</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F17">
         <v>64</v>
@@ -1154,27 +1184,24 @@
         <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I17" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>2619</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F18">
         <v>23</v>
@@ -1183,27 +1210,24 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I18" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>2620</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>93</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F19">
         <v>26</v>
@@ -1212,27 +1236,27 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>3574</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F20">
         <v>26</v>
@@ -1241,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="J20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1259,11 +1283,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1289,67 +1315,67 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1361,11 +1387,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1391,49 +1419,49 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>